<commit_message>
upd xlsx for lab 28
</commit_message>
<xml_diff>
--- a/lab28/Лаб28_Исследование сортировок.xlsx
+++ b/lab28/Лаб28_Исследование сортировок.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying ULSTU\1 курс\ОАиП\Мои Лабы\lab28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBCF56A-C912-4941-A112-C6F8FC9C7C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE865B9-C19E-4733-B6FC-809A0500F13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D6F89E9D-65BC-42F3-8914-22659B734967}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6F89E9D-65BC-42F3-8914-22659B734967}"/>
   </bookViews>
   <sheets>
     <sheet name="Сводная" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>dict0.txt</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Shell</t>
+  </si>
+  <si>
+    <t>Есть очень много сортировок, и они все могут быть эффективны</t>
+  </si>
+  <si>
+    <t>Написать сортировку самому, опираясь на код из интернета</t>
+  </si>
+  <si>
+    <t>Выбор метода сортировки зависит от конкретной задачи</t>
   </si>
 </sst>
 </file>
@@ -277,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -297,6 +306,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEAEE42-FA95-47D1-8B01-CA3ED8371D4E}">
   <dimension ref="B1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,19 +721,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>35</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1005,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BBB95-4CF1-426E-8849-FEDB3A6D33E6}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>

</xml_diff>